<commit_message>
Started coding the Lexical Analyzer
</commit_message>
<xml_diff>
--- a/doc/Instruções.xlsx
+++ b/doc/Instruções.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="48">
   <si>
     <t>Instruções</t>
   </si>
@@ -136,6 +136,30 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Opcode</t>
+  </si>
+  <si>
+    <t>Funct</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>0x00</t>
+  </si>
+  <si>
+    <t>0x20</t>
+  </si>
+  <si>
+    <t>0x60</t>
+  </si>
+  <si>
+    <t>Reg, Reg, Reg</t>
   </si>
 </sst>
 </file>
@@ -623,27 +647,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F45"/>
+  <dimension ref="A2:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="40.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="40.7109375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:5" s="6" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:8" s="6" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
@@ -654,20 +678,42 @@
         <v>2</v>
       </c>
       <c r="E4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -676,8 +722,11 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -686,8 +735,11 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
@@ -696,8 +748,11 @@
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
@@ -706,8 +761,11 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
@@ -716,8 +774,11 @@
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
@@ -726,8 +787,11 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
@@ -736,8 +800,11 @@
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
@@ -746,8 +813,11 @@
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
@@ -756,8 +826,11 @@
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
@@ -766,8 +839,11 @@
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
@@ -776,14 +852,17 @@
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-    </row>
-    <row r="19" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="19" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B19" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="2:5" s="6" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="2:8" s="6" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>0</v>
       </c>
@@ -793,11 +872,14 @@
       <c r="D21" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
@@ -806,8 +888,11 @@
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
@@ -816,8 +901,11 @@
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
@@ -826,8 +914,11 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
@@ -836,8 +927,11 @@
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
@@ -846,8 +940,11 @@
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
@@ -856,8 +953,11 @@
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
@@ -866,8 +966,11 @@
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
@@ -876,8 +979,11 @@
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
@@ -886,8 +992,11 @@
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>31</v>
       </c>
@@ -896,8 +1005,11 @@
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>32</v>
       </c>
@@ -906,8 +1018,11 @@
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
@@ -916,8 +1031,11 @@
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>38</v>
       </c>
@@ -926,8 +1044,11 @@
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>34</v>
       </c>
@@ -936,8 +1057,11 @@
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>35</v>
       </c>
@@ -946,8 +1070,11 @@
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>36</v>
       </c>
@@ -956,8 +1083,11 @@
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
-    </row>
-    <row r="38" spans="1:6" s="6" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="4" t="s">
         <v>37</v>
       </c>
@@ -966,14 +1096,17 @@
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
-    </row>
-    <row r="41" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="41" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="B41" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
       <c r="B43" s="7" t="s">
         <v>0</v>
@@ -984,26 +1117,35 @@
       <c r="D43" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F43" s="6"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improved the Lexical Analyzer (not ready). Need to treat immediates in any format (binary, octal, decimal, hexadecimal)
</commit_message>
<xml_diff>
--- a/doc/Instruções.xlsx
+++ b/doc/Instruções.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
   <si>
     <t>Instruções</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Funct</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
   </si>
   <si>
     <t>0x20</t>
-  </si>
-  <si>
-    <t>0x60</t>
   </si>
   <si>
     <t>Reg, Reg, Reg</t>
@@ -647,27 +641,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I45"/>
+  <dimension ref="A2:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12.7109375" style="1" customWidth="1"/>
-    <col min="3" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="40.7109375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="40.7109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:8" s="6" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:7" s="6" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
@@ -684,13 +678,10 @@
         <v>41</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -698,22 +689,19 @@
         <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -724,9 +712,8 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -737,9 +724,8 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
@@ -750,9 +736,8 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
@@ -763,9 +748,8 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>4</v>
       </c>
@@ -776,9 +760,8 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
@@ -789,9 +772,8 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
@@ -802,9 +784,8 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
@@ -815,9 +796,8 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
@@ -828,9 +808,8 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
@@ -841,9 +820,8 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
@@ -854,15 +832,14 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="19" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="2:7" ht="21" x14ac:dyDescent="0.35">
       <c r="B19" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="2:8" s="6" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="2:7" s="6" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>0</v>
       </c>
@@ -874,12 +851,11 @@
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8" t="s">
+      <c r="G21" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
@@ -890,9 +866,8 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
@@ -903,9 +878,8 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
@@ -916,9 +890,8 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
@@ -929,9 +902,8 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
@@ -942,9 +914,8 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
@@ -955,9 +926,8 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
@@ -968,9 +938,8 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
@@ -981,9 +950,8 @@
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
@@ -994,9 +962,8 @@
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>31</v>
       </c>
@@ -1007,9 +974,8 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>32</v>
       </c>
@@ -1020,9 +986,8 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
@@ -1033,9 +998,8 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>38</v>
       </c>
@@ -1046,9 +1010,8 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>34</v>
       </c>
@@ -1059,9 +1022,8 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>35</v>
       </c>
@@ -1072,9 +1034,8 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>36</v>
       </c>
@@ -1085,9 +1046,8 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-    </row>
-    <row r="38" spans="1:9" s="6" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:8" s="6" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="4" t="s">
         <v>37</v>
       </c>
@@ -1098,15 +1058,14 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-    </row>
-    <row r="41" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B41" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
       <c r="B43" s="7" t="s">
         <v>0</v>
@@ -1119,13 +1078,12 @@
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8" t="s">
+      <c r="G43" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="I43" s="6"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>39</v>
       </c>
@@ -1134,9 +1092,8 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="4" t="s">
         <v>39</v>
       </c>
@@ -1145,7 +1102,6 @@
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the file "Instruções.xlsx". Instructions were classified in 8 subtypes according to their required operands
</commit_message>
<xml_diff>
--- a/doc/Instruções.xlsx
+++ b/doc/Instruções.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="99">
   <si>
     <t>Instruções</t>
   </si>
@@ -96,12 +96,6 @@
     <t>bne</t>
   </si>
   <si>
-    <t>lbu</t>
-  </si>
-  <si>
-    <t>lhu</t>
-  </si>
-  <si>
     <t>lui</t>
   </si>
   <si>
@@ -162,9 +156,6 @@
     <t>I2</t>
   </si>
   <si>
-    <t>J2</t>
-  </si>
-  <si>
     <t>I1</t>
   </si>
   <si>
@@ -216,68 +207,119 @@
     <t>Imm</t>
   </si>
   <si>
-    <t>000000b</t>
-  </si>
-  <si>
-    <t>100010b</t>
-  </si>
-  <si>
-    <t>1000100b</t>
-  </si>
-  <si>
-    <t>100101b</t>
-  </si>
-  <si>
-    <t>001000b</t>
-  </si>
-  <si>
     <t>Null</t>
   </si>
   <si>
-    <t>100011b</t>
-  </si>
-  <si>
-    <t>101011b</t>
-  </si>
-  <si>
-    <t>000100b</t>
-  </si>
-  <si>
-    <t>000010b</t>
-  </si>
-  <si>
-    <t>000011b</t>
-  </si>
-  <si>
-    <t>Reg,Reg, Reg, Shant</t>
-  </si>
-  <si>
     <t>Reg, Reg, Imm</t>
   </si>
   <si>
     <t>I3</t>
   </si>
   <si>
-    <t>offset&lt;&lt;2</t>
-  </si>
-  <si>
-    <t>Target&lt;&lt;2</t>
-  </si>
-  <si>
     <t>Reg</t>
   </si>
   <si>
-    <t>nextPC&lt;-Reg</t>
-  </si>
-  <si>
-    <t>$ra &lt;- PC+8 ou nextPC + 4</t>
+    <t>0x02</t>
+  </si>
+  <si>
+    <t>0x03</t>
+  </si>
+  <si>
+    <t>0x08</t>
+  </si>
+  <si>
+    <t>0x23</t>
+  </si>
+  <si>
+    <t>0x2B</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>0x22</t>
+  </si>
+  <si>
+    <t>0x25</t>
+  </si>
+  <si>
+    <t>0x24</t>
+  </si>
+  <si>
+    <t>Reg, Imm_opt, Reg</t>
+  </si>
+  <si>
+    <t>Reg, Reg, Label</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>0x05</t>
+  </si>
+  <si>
+    <t>Reg, Imm</t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+  <si>
+    <t>lh</t>
+  </si>
+  <si>
+    <t>I4</t>
+  </si>
+  <si>
+    <t>0x21</t>
+  </si>
+  <si>
+    <t>0x27</t>
+  </si>
+  <si>
+    <t>0x2A</t>
+  </si>
+  <si>
+    <t>0x09</t>
+  </si>
+  <si>
+    <t>0x0C</t>
+  </si>
+  <si>
+    <t>0x0D</t>
+  </si>
+  <si>
+    <t>0x0A</t>
+  </si>
+  <si>
+    <t>0x0B</t>
+  </si>
+  <si>
+    <t>0x0F</t>
+  </si>
+  <si>
+    <t>0x28</t>
+  </si>
+  <si>
+    <t>0x29</t>
+  </si>
+  <si>
+    <t>Gramática</t>
+  </si>
+  <si>
+    <t>Sintaxe</t>
+  </si>
+  <si>
+    <t>Mapa de Memória</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,7 +344,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -415,11 +457,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -457,6 +510,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,9 +539,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -512,7 +579,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -546,6 +613,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -580,9 +648,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -755,14 +824,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:I59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:N72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21:N41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12.7109375" style="1" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="1"/>
@@ -772,13 +841,13 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="21">
+    <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15.75" thickBot="1"/>
-    <row r="4" spans="2:9" s="6" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:8" s="6" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
@@ -789,16 +858,16 @@
         <v>2</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
@@ -806,19 +875,19 @@
         <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9">
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -826,19 +895,19 @@
         <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -846,19 +915,19 @@
         <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
@@ -866,19 +935,19 @@
         <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
@@ -886,148 +955,141 @@
         <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9">
-      <c r="B10" s="2" t="s">
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9">
-      <c r="B11" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9">
-      <c r="B15" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="15.75" thickBot="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
@@ -1035,31 +1097,25 @@
         <v>17</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="21">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B19" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="15.75" thickBot="1"/>
-    <row r="21" spans="2:7" s="6" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="20" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:14" s="6" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>0</v>
       </c>
@@ -1069,223 +1125,368 @@
       <c r="D21" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
+      <c r="E21" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="G21" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="2:7">
+        <v>15</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="2:7">
+      <c r="D23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="2:7">
+        <v>15</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="2:7">
+        <v>15</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="2:7">
+        <v>15</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
       <c r="B27" s="2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="2:7">
+        <v>15</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="2:7">
+      <c r="D28" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="2:7">
+        <v>16</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="2:7">
+      <c r="D30" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="2:7">
+        <v>16</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="D32" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="D33" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:8">
+        <v>16</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="1:8">
+        <v>16</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="D36" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="1:8" s="6" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="D37" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" s="6" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-    </row>
-    <row r="41" spans="1:8" ht="21">
+        <v>16</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+    </row>
+    <row r="41" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="B41" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15.75" thickBot="1"/>
-    <row r="43" spans="1:8" ht="15.75" thickBot="1">
+    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
       <c r="B43" s="7" t="s">
         <v>0</v>
@@ -1303,9 +1504,9 @@
       </c>
       <c r="H43" s="6"/>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="3"/>
@@ -1313,9 +1514,9 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:8" ht="15.75" thickBot="1">
+    <row r="45" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="5"/>
@@ -1323,197 +1524,286 @@
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
     </row>
-    <row r="50" spans="2:8">
+    <row r="48" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="B48" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D50" s="16"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C59" s="13"/>
+    </row>
+    <row r="61" spans="2:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B61" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="51" spans="2:8">
-      <c r="B51" s="1" t="s">
+      <c r="C66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F51" s="1" t="s">
+      <c r="C68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G51" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8">
-      <c r="B52" s="1" t="s">
+      <c r="G68" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F52" s="1" t="s">
+      <c r="C69" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8">
-      <c r="B53" s="1" t="s">
+      <c r="G69" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F53" s="1" t="s">
+      <c r="C71" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G53" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8">
-      <c r="B55" s="1" t="s">
+      <c r="E71" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8">
-      <c r="B56" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8">
-      <c r="B58" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8">
-      <c r="B59" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>65</v>
+      <c r="D72" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C50:D50"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>